<commit_message>
add new Q&A for question generation feature
</commit_message>
<xml_diff>
--- a/data/examples.xlsx
+++ b/data/examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spicy/Nutstore Files/我的坚果云/拓展/拓展桌面/助教机器人/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candice/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825D7E4-6687-C548-88B3-6F1C9F6B7646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A94B8-AF86-F743-82BD-DFA710C96A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{70C9AA9B-C874-4140-A988-75F7910597F0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="17700" xr2:uid="{70C9AA9B-C874-4140-A988-75F7910597F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>什么是合成生物学？</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -391,12 +391,69 @@
     <t>5.2.3.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>很好，这是一个不错的尝试！但未来合成科学的发展方向不仅包括新材料和生物燃料。化学合成与生物合成之间的交叉互融将主要围绕催化剂、反应、合成策略和功能分子等四个层次的多个方向展开。主要发展方向包括：生物合成的分子机制的研究、仿生催化体系的发展和创新、仿生反应的发展和创新、复杂天然产物的仿生合成、人工酶的发展和应用、酶催化反应驱动活性分子合成、生物分子糖、蛋白质和核酸的合成、生物促进的合成化学策略的开发和运用。继续探索这些方面，你会发现合成科学的无限可能性！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请帮我出一个新的题目吧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好的，我很高兴看到你的学习热情！请问合成科学的新特点是什么？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不太正确哦！合成科学的新特点除了提高效率外，还涉及到一个更广泛的方面。想一想，合成科学如何能够在绿色合成和新功能分子设计方面发挥作用？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以使物质合成更加绿色？帮助新功能分子的设计和合成？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很好！合成化学和生物合成的交叉互融与相互促进推动了合成科学的变革和发展。新特点和新挑战包括：使物质合成更加绿色、高效，有助于解决传统合成难以解决的环境、效率和生态问题；使合成的手段更加丰富，有望解决合成中的重大战略问题；有助于更多、更好的新功能分子的设计与合成，满足和促进多个领域的发展与创新；充分发挥化学合成和生物合成各自的优势，助力我国物质科学相关领域创新、发展和产业升级。
+如果你需要更多的题目或者其他类型的帮助，请随时告诉我！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好的，请问化学促进的生物合成是什么？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>化学促进的生物合成的本质是发生在生物体系中的合成化学过程，研究对象通常为天然存在的功能分子。它利用各种酶促反应，完成化学结构的逐步构筑过程，体现在基因、蛋白质（酶）、细胞、反应、途径等不同层次。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非常好！你成功阐述了化学促进的生物合成的本质。如果你需要更多的题目或者其他类型的帮助，请随时告诉我！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好的，请问合成科学的未来发展方向包括哪些？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请帮我出一些关于合成科学的题目吧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未来合成科学的发展方向主要在于发展新的合成材料和生物燃料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成科学的新特点是提高合成效率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我想要更多的题目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -427,6 +484,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -450,7 +514,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -459,6 +523,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,9 +545,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -518,7 +585,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -624,7 +691,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -766,7 +833,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -774,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E5B596-07D8-904F-8861-9EDC766CED2D}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="119" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1130,6 +1197,83 @@
         <v>69</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="34">
+      <c r="A32">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="255">
+      <c r="A33">
+        <v>23</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="34">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="85">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="255">
+      <c r="A36">
+        <v>26</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="34">
+      <c r="A37">
+        <v>27</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="119">
+      <c r="A38">
+        <v>28</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>